<commit_message>
Created Spaghetti Creator and coded 2 tables
</commit_message>
<xml_diff>
--- a/SpaghettiPlan.xlsx
+++ b/SpaghettiPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University Projects\CSE-609-Data-Analytics-and-Warehousing\dawh-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA Course Material\CSE 609 - Data Analytics and Warehousing\Semester Project\dawh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E62B43-BB17-4159-AD88-768D3D52EF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101B2F50-853C-4D28-9EFE-324E73F8989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="116">
   <si>
     <t>Source Table Name</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>Might need Normalization</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>"DIAG-"FactTablePK</t>
+  </si>
+  <si>
+    <t>"SERV-"FactTablePK</t>
+  </si>
+  <si>
+    <t>dimDateServicePK</t>
+  </si>
+  <si>
+    <t>MIN(dimDateServicePK) - RAND(10)</t>
+  </si>
+  <si>
+    <t>Generated using Faker</t>
   </si>
 </sst>
 </file>
@@ -386,7 +404,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -409,17 +427,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF962305-B2DA-41D2-A53B-7757C2B34C97}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,9 +778,10 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -765,15 +797,19 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
@@ -787,8 +823,9 @@
         <v>4</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -802,8 +839,9 @@
         <v>10</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
@@ -817,8 +855,9 @@
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -832,8 +871,9 @@
         <v>6</v>
       </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -847,34 +887,49 @@
         <v>40</v>
       </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -888,8 +943,9 @@
         <v>12</v>
       </c>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -903,8 +959,9 @@
         <v>13</v>
       </c>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -918,15 +975,17 @@
         <v>14</v>
       </c>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -940,21 +999,29 @@
         <v>5</v>
       </c>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
       <c r="E15" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -968,8 +1035,9 @@
         <v>16</v>
       </c>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -983,8 +1051,9 @@
         <v>17</v>
       </c>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
@@ -998,8 +1067,9 @@
         <v>18</v>
       </c>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>62</v>
       </c>
@@ -1013,8 +1083,9 @@
         <v>19</v>
       </c>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1028,8 +1099,9 @@
         <v>21</v>
       </c>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
@@ -1043,8 +1115,9 @@
         <v>81</v>
       </c>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
@@ -1056,8 +1129,11 @@
       <c r="E22" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
@@ -1069,8 +1145,11 @@
       <c r="E23" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1084,8 +1163,9 @@
         <v>29</v>
       </c>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>62</v>
       </c>
@@ -1099,8 +1179,9 @@
         <v>30</v>
       </c>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
@@ -1114,15 +1195,17 @@
         <v>28</v>
       </c>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
@@ -1136,8 +1219,9 @@
         <v>16</v>
       </c>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>72</v>
       </c>
@@ -1149,8 +1233,9 @@
       <c r="E29" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>72</v>
       </c>
@@ -1164,8 +1249,9 @@
         <v>22</v>
       </c>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -1181,8 +1267,9 @@
       <c r="E31" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
@@ -1194,8 +1281,9 @@
       <c r="E32" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>72</v>
       </c>
@@ -1207,8 +1295,9 @@
       <c r="E33" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1222,8 +1311,9 @@
         <v>23</v>
       </c>
       <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>72</v>
       </c>
@@ -1237,8 +1327,9 @@
         <v>24</v>
       </c>
       <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -1252,8 +1343,9 @@
         <v>25</v>
       </c>
       <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -1267,8 +1359,9 @@
         <v>26</v>
       </c>
       <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>72</v>
       </c>
@@ -1282,14 +1375,16 @@
         <v>27</v>
       </c>
       <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>86</v>
       </c>
@@ -1303,8 +1398,9 @@
         <v>6</v>
       </c>
       <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>86</v>
       </c>
@@ -1318,8 +1414,9 @@
         <v>32</v>
       </c>
       <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>86</v>
       </c>
@@ -1331,8 +1428,9 @@
       <c r="E42" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -1348,8 +1446,9 @@
       <c r="E43" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -1361,8 +1460,9 @@
       <c r="E44" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
@@ -1378,8 +1478,9 @@
       <c r="E45" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>86</v>
       </c>
@@ -1393,8 +1494,9 @@
         <v>35</v>
       </c>
       <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>86</v>
       </c>
@@ -1408,8 +1510,9 @@
         <v>37</v>
       </c>
       <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>86</v>
       </c>
@@ -1423,15 +1526,17 @@
         <v>104</v>
       </c>
       <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>37</v>
       </c>
@@ -1445,8 +1550,9 @@
         <v>104</v>
       </c>
       <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>37</v>
       </c>
@@ -1460,8 +1566,9 @@
         <v>37</v>
       </c>
       <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
@@ -1475,8 +1582,9 @@
         <v>38</v>
       </c>
       <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>37</v>
       </c>
@@ -1490,15 +1598,17 @@
         <v>105</v>
       </c>
       <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>90</v>
       </c>
@@ -1512,8 +1622,9 @@
         <v>7</v>
       </c>
       <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>90</v>
       </c>
@@ -1527,8 +1638,9 @@
         <v>40</v>
       </c>
       <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>90</v>
       </c>
@@ -1540,8 +1652,9 @@
       <c r="E57" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>90</v>
       </c>
@@ -1553,8 +1666,9 @@
       <c r="E58" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>90</v>
       </c>
@@ -1566,8 +1680,9 @@
       <c r="E59" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>90</v>
       </c>
@@ -1579,8 +1694,9 @@
       <c r="E60" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>90</v>
       </c>
@@ -1592,15 +1708,17 @@
       <c r="E61" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>94</v>
       </c>
@@ -1612,8 +1730,9 @@
       <c r="E63" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>94</v>
       </c>
@@ -1627,8 +1746,9 @@
         <v>5</v>
       </c>
       <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>94</v>
       </c>
@@ -1642,8 +1762,9 @@
         <v>6</v>
       </c>
       <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>94</v>
       </c>
@@ -1655,8 +1776,9 @@
       <c r="E66" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>94</v>
       </c>
@@ -1668,8 +1790,9 @@
       <c r="E67" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>94</v>
       </c>
@@ -1681,8 +1804,9 @@
       <c r="E68" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>94</v>
       </c>
@@ -1698,8 +1822,9 @@
       <c r="E69" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>94</v>
       </c>
@@ -1713,8 +1838,9 @@
         <v>11</v>
       </c>
       <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>94</v>
       </c>
@@ -1730,15 +1856,17 @@
       <c r="E71" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>99</v>
       </c>
@@ -1752,8 +1880,9 @@
         <v>47</v>
       </c>
       <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>99</v>
       </c>
@@ -1767,8 +1896,9 @@
         <v>49</v>
       </c>
       <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>99</v>
       </c>
@@ -1782,15 +1912,17 @@
         <v>48</v>
       </c>
       <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -1804,8 +1936,9 @@
         <v>42</v>
       </c>
       <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>100</v>
       </c>
@@ -1819,8 +1952,9 @@
         <v>44</v>
       </c>
       <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>100</v>
       </c>
@@ -1834,8 +1968,10 @@
         <v>43</v>
       </c>
       <c r="E79" s="2"/>
+      <c r="F79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated and ran Sphaghetti creater
</commit_message>
<xml_diff>
--- a/SpaghettiPlan.xlsx
+++ b/SpaghettiPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA Course Material\CSE 609 - Data Analytics and Warehousing\Semester Project\dawh-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University Projects\CSE-609-Data-Analytics-and-Warehousing\dawh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7F91C9-708B-4203-BCE0-FBCD7545DB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701753AD-11DD-42AC-AB4D-22DCB5D695E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="124">
   <si>
     <t>Source Table Name</t>
   </si>
@@ -62,9 +51,6 @@
     <t>dimLocationPK</t>
   </si>
   <si>
-    <t>dimCPTCodePK</t>
-  </si>
-  <si>
     <t>dimDatePostPK</t>
   </si>
   <si>
@@ -341,15 +327,9 @@
     <t>SpecialityDesc</t>
   </si>
   <si>
-    <t>Needs to be Generated.Will contain either Diagnostic Report or Service Report.</t>
-  </si>
-  <si>
     <t>ApprovingDoctorNbr</t>
   </si>
   <si>
-    <t>Might need Normalization</t>
-  </si>
-  <si>
     <t>Formula</t>
   </si>
   <si>
@@ -378,6 +358,45 @@
   </si>
   <si>
     <t>GeneratedDate</t>
+  </si>
+  <si>
+    <t>MIN(RegistrationDate) - RAND(3)</t>
+  </si>
+  <si>
+    <t>NORMAL DISTRIBUTION (150, 20)</t>
+  </si>
+  <si>
+    <t>WeightLbs * 0.453592</t>
+  </si>
+  <si>
+    <t>LOWER(FirstName).LOWER(LastName)@datacourse.com</t>
+  </si>
+  <si>
+    <t>IF LastName CONTAINS "Dr. " THEN 'Dr.'</t>
+  </si>
+  <si>
+    <t>REPLACE "Dr. " WITH ""</t>
+  </si>
+  <si>
+    <t>dimDateServicePK for DiagnosisReport, dimDatePostPK for ServiceReport</t>
+  </si>
+  <si>
+    <t>FactTablePK for DiagnosisReport, FactTablePK + 210964322 for ServiceReport</t>
+  </si>
+  <si>
+    <t>"DIAG-"FactTablePK for DiagnosisReport, "SERV-"FactTablePK for ServiceReport</t>
+  </si>
+  <si>
+    <t>"Diagnosis" for DiagnosisReport, "Service" for ServiceReport</t>
+  </si>
+  <si>
+    <t>Generated using base64</t>
+  </si>
+  <si>
+    <t>Null for DiagnosisReport</t>
+  </si>
+  <si>
+    <t>Null for ServiceReport</t>
   </si>
 </sst>
 </file>
@@ -447,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -455,6 +474,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,26 +792,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF962305-B2DA-41D2-A53B-7757C2B34C97}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -802,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,14 +832,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -827,30 +848,30 @@
         <v>4</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -859,14 +880,14 @@
         <v>5</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -875,30 +896,30 @@
         <v>6</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
@@ -907,18 +928,18 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>105</v>
+        <v>67</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -927,59 +948,59 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>106</v>
+        <v>67</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -987,219 +1008,219 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>108</v>
+        <v>67</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1207,330 +1228,348 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
       <c r="E29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="2"/>
-      <c r="F36" s="1"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="1"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E38" s="2"/>
-      <c r="F38" s="1"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="1"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="s">
         <v>30</v>
       </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E46" s="2"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E47" s="2"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -1538,71 +1577,71 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="1"/>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E50" s="2"/>
-      <c r="F50" s="1"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C52" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E53" s="2"/>
-      <c r="F53" s="1"/>
+      <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
@@ -1610,121 +1649,125 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="1"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E55" s="2"/>
-      <c r="F55" s="1"/>
+      <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E56" s="2"/>
-      <c r="F56" s="1"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F57" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F58" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
@@ -1732,42 +1775,46 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="65" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>3</v>
@@ -1776,14 +1823,14 @@
         <v>5</v>
       </c>
       <c r="E65" s="2"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>3</v>
@@ -1792,101 +1839,109 @@
         <v>6</v>
       </c>
       <c r="E66" s="2"/>
-      <c r="F66" s="1"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F68" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F69" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F70" s="1"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E71" s="2"/>
-      <c r="F71" s="1"/>
+      <c r="F71" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="1"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
@@ -1894,55 +1949,55 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
-      <c r="F73" s="1"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="F74" s="1"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E75" s="2"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E76" s="2"/>
-      <c r="F76" s="1"/>
+      <c r="F76" s="5"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
@@ -1950,55 +2005,55 @@
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E78" s="2"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="C79" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E79" s="2"/>
-      <c r="F79" s="1"/>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E80" s="2"/>
-      <c r="F80" s="1"/>
+      <c r="F80" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated and ran Sphaghetti creater, updated StarSchemaPlan.xlsx
</commit_message>
<xml_diff>
--- a/SpaghettiPlan.xlsx
+++ b/SpaghettiPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University Projects\CSE-609-Data-Analytics-and-Warehousing\dawh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6494911C-F625-4071-B907-127EFEDE3FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1212F66E-11E9-4BFD-AB50-99B7789ECC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="128">
   <si>
     <t>Source Table Name</t>
   </si>
@@ -378,9 +378,6 @@
     <t>REPLACE "Dr. " WITH ""</t>
   </si>
   <si>
-    <t>dimDateServicePK for DiagnosisReport, dimDatePostPK for ServiceReport</t>
-  </si>
-  <si>
     <t>FactTablePK for DiagnosisReport, FactTablePK + 210964322 for ServiceReport</t>
   </si>
   <si>
@@ -397,6 +394,21 @@
   </si>
   <si>
     <t>Null for ServiceReport</t>
+  </si>
+  <si>
+    <t>dimDateServicePK - RAND(10) for DiagnosisReport, dimDateServicePK for ServiceReport</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>State Code</t>
   </si>
 </sst>
 </file>
@@ -420,12 +432,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -466,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -474,6 +492,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF962305-B2DA-41D2-A53B-7757C2B34C97}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +820,7 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,77 +1224,73 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="A27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1285,95 +1300,99 @@
         <v>70</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>104</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1383,13 +1402,13 @@
         <v>70</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1399,126 +1418,118 @@
         <v>70</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="A41" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>114</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1526,102 +1537,110 @@
         <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
@@ -1630,105 +1649,103 @@
         <v>35</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>109</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E59" s="2"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,106 +1753,110 @@
         <v>84</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F60" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="D62" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E63" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>118</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E64" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
@@ -1844,7 +1865,7 @@
         <v>88</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -1852,7 +1873,7 @@
         <v>67</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,7 +1881,7 @@
         <v>88</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -1868,59 +1889,55 @@
         <v>67</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>121</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E70" s="2"/>
-      <c r="F70" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F71" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1928,33 +1945,39 @@
         <v>88</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F72" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
+      <c r="A73" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>43</v>
@@ -1963,39 +1986,45 @@
         <v>45</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>47</v>
+        <v>3</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
+      <c r="F75" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
@@ -2007,51 +2036,107 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created DAG and Other Files
</commit_message>
<xml_diff>
--- a/SpaghettiPlan.xlsx
+++ b/SpaghettiPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA Course Material\CSE 609 - Data Analytics and Warehousing\Semester Project\dawh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E4DCE4-24D9-40C3-87FF-B541D27C1F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EC07C9-C4F0-4C8E-AD4B-E68240BF1BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{782874DB-19AE-4872-A413-142EA3722F57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,9 +360,6 @@
     <t>GeneratedDate</t>
   </si>
   <si>
-    <t>MIN(RegistrationDate) - RAND(3)</t>
-  </si>
-  <si>
     <t>NORMAL DISTRIBUTION (150, 20)</t>
   </si>
   <si>
@@ -448,6 +445,9 @@
   </si>
   <si>
     <t>Daily, Weekly, Bi-Weekly, Monthly, Occasionally</t>
+  </si>
+  <si>
+    <t>MIN(RegistrationDate) + RAND(3)</t>
   </si>
 </sst>
 </file>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF962305-B2DA-41D2-A53B-7757C2B34C97}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
         <v>101</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H17" s="6">
         <v>0.04</v>
@@ -1176,7 +1176,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H18" s="6">
         <v>0.06</v>
@@ -1215,7 +1215,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H20" s="6">
         <v>1</v>
@@ -1305,7 +1305,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="6">
         <v>0.1</v>
@@ -1316,18 +1316,18 @@
         <v>60</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="6">
         <v>0.3</v>
@@ -1338,19 +1338,19 @@
         <v>60</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="2"/>
       <c r="H27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>70</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>13</v>
@@ -1413,7 +1413,7 @@
         <v>67</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="G31" s="2"/>
     </row>
@@ -1433,7 +1433,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H32" s="6">
         <v>0.35</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H33" s="6">
         <v>0.05</v>
@@ -1476,10 +1476,10 @@
         <v>67</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H34" s="6">
         <v>0.1</v>
@@ -1498,10 +1498,10 @@
         <v>67</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H35" s="6">
         <v>0.45</v>
@@ -1574,7 +1574,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H39" s="6">
         <v>1</v>
@@ -1602,13 +1602,13 @@
         <v>70</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1690,7 +1690,7 @@
         <v>97</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G46" s="2"/>
     </row>
@@ -1707,7 +1707,7 @@
         <v>67</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G47" s="2"/>
     </row>
@@ -1728,7 +1728,7 @@
         <v>97</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G48" s="2"/>
     </row>
@@ -1999,13 +1999,13 @@
         <v>84</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>109</v>
@@ -2035,7 +2035,7 @@
         <v>67</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G67" s="2"/>
     </row>
@@ -2052,7 +2052,7 @@
         <v>67</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G68" s="2"/>
     </row>
@@ -2103,7 +2103,7 @@
         <v>67</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G71" s="2"/>
     </row>
@@ -2120,7 +2120,7 @@
         <v>67</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G72" s="2"/>
     </row>
@@ -2137,7 +2137,7 @@
         <v>67</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G73" s="2"/>
     </row>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G74" s="2"/>
     </row>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G75" s="2"/>
     </row>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G76" s="2"/>
     </row>

</xml_diff>